<commit_message>
DONE: SWC-MODE-SWITCH-EVENT is now treated as PER event type TODO: improve offset computing algo
</commit_message>
<xml_diff>
--- a/RTE_Configurator test plan.xlsx
+++ b/RTE_Configurator test plan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristi\PycharmProjects\RTE_Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
   </bookViews>
@@ -11,11 +16,11 @@
     <sheet name="Overview" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Overview!$A$1:$E$27</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="101">
   <si>
     <t>Requirements</t>
   </si>
@@ -903,13 +908,39 @@
       </rPr>
       <t>: Provide to the tool one arxml file that contains three events (event1 of type SWC-MODE-SWITCH-EVENT , event2 of type DATA-RECEIVED-EVENT and event 3 of type SWC-MODE-SWITCH-EVENT). The event1 one will have ACTIVATION = ON-ENTRY, while the event 3 will have ACTIVATION = ON-EXIT, and all the three events will be mapped on the same task</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 5:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Provide to the tool one arxml file which contains one TIMING-EVENT,  and one allocation file, which has the CORE and PARTITION parameters set for the existing swc component that references the SWC-MODE-SWITCH-EVENT </t>
+    </r>
+  </si>
+  <si>
+    <t>- check that the SWC-MODE-SWITCH-EVENT is present in the script, and it's RteMappedToTaskRef parameter has the correct form: TaskApp_CORE_PARTITION_PER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -971,7 +1002,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1216,11 +1247,72 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1302,12 +1394,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1332,6 +1418,30 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1706,28 +1816,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
@@ -1741,7 +1851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -1755,97 +1865,97 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="17"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -1858,17 +1968,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
@@ -1878,7 +1988,7 @@
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -1898,7 +2008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30.75" thickTop="1">
+    <row r="2" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>29</v>
       </c>
@@ -1918,7 +2028,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>30</v>
       </c>
@@ -1938,7 +2048,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>31</v>
       </c>
@@ -1958,7 +2068,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>34</v>
       </c>
@@ -1978,11 +2088,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="45" t="s">
         <v>43</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1997,11 +2107,11 @@
       <c r="F6" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="37"/>
-    </row>
-    <row r="7" spans="1:7" ht="60">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
+      <c r="G6" s="35"/>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="44"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="18" t="s">
         <v>46</v>
       </c>
@@ -2015,9 +2125,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="44"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="18" t="s">
         <v>47</v>
       </c>
@@ -2031,9 +2141,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="44"/>
+      <c r="B9" s="45"/>
       <c r="C9" s="18" t="s">
         <v>48</v>
       </c>
@@ -2047,7 +2157,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>49</v>
       </c>
@@ -2067,7 +2177,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>51</v>
       </c>
@@ -2087,7 +2197,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
         <v>55</v>
       </c>
@@ -2107,11 +2217,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="45">
-      <c r="A13" s="35" t="s">
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="45" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="18" t="s">
@@ -2127,9 +2237,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="44"/>
+      <c r="B14" s="45"/>
       <c r="C14" s="18" t="s">
         <v>63</v>
       </c>
@@ -2143,9 +2253,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="45">
-      <c r="A15" s="35"/>
-      <c r="B15" s="36"/>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="C15" s="18" t="s">
         <v>64</v>
       </c>
@@ -2159,9 +2269,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30">
-      <c r="A16" s="35"/>
-      <c r="B16" s="36"/>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="C16" s="18" t="s">
         <v>65</v>
       </c>
@@ -2175,9 +2285,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="44"/>
+      <c r="B17" s="45"/>
       <c r="C17" s="18" t="s">
         <v>66</v>
       </c>
@@ -2191,11 +2301,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60">
-      <c r="A18" s="35" t="s">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="49" t="s">
         <v>68</v>
       </c>
       <c r="C18" s="18" t="s">
@@ -2211,9 +2321,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="60">
-      <c r="A19" s="35"/>
-      <c r="B19" s="36"/>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="47"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="18" t="s">
         <v>96</v>
       </c>
@@ -2227,10 +2337,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="75">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="45" t="s">
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="47"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="43" t="s">
         <v>97</v>
       </c>
       <c r="D20" s="25" t="s">
@@ -2243,9 +2353,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="75">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36"/>
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="18" t="s">
         <v>71</v>
       </c>
@@ -2259,176 +2369,192 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45">
-      <c r="A22" s="35" t="s">
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="48"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B23" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C23" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D23" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45">
-      <c r="A23" s="35"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="18" t="s">
+      <c r="E23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D24" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45">
-      <c r="A24" s="35"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="18" t="s">
+      <c r="E24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="44"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D25" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" ht="45">
-      <c r="A25" s="26" t="s">
+      <c r="E25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B26" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D25" s="27" t="s">
+      <c r="D26" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30">
-      <c r="A26" s="26" t="s">
+      <c r="E26" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B27" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C27" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D27" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="75">
-      <c r="A27" s="26" t="s">
+      <c r="E27" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A28" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B28" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C28" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D28" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30">
-      <c r="A28" s="38" t="s">
+      <c r="E28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B29" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C29" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D29" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30.75" thickBot="1">
-      <c r="A29" s="39" t="s">
+      <c r="E29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B30" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C30" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="42" t="s">
+      <c r="D30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="43" t="s">
+      <c r="E30" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="44" t="s">
+      <c r="F30" s="42" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="B31" s="1" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>95</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E26"/>
+  <autoFilter ref="A1:E27"/>
   <mergeCells count="8">
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
-  <conditionalFormatting sqref="E25:E1048576 E1:E21">
+  <conditionalFormatting sqref="E26:E1048576 E1:E22">
     <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"done"</formula>
     </cfRule>
@@ -2436,7 +2562,7 @@
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:F29 F2:F21">
+  <conditionalFormatting sqref="F26:F30 F2:F22">
     <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
@@ -2444,12 +2570,12 @@
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F25:F29 F2:F21">
+  <conditionalFormatting sqref="F26:F30 F2:F22">
     <cfRule type="cellIs" dxfId="5" priority="17" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E24">
+  <conditionalFormatting sqref="E23:E25">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"done"</formula>
     </cfRule>
@@ -2457,7 +2583,7 @@
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F24">
+  <conditionalFormatting sqref="F23:F25">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
@@ -2465,16 +2591,16 @@
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22:F24">
+  <conditionalFormatting sqref="F23:F25">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E30">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F30">
       <formula1>"YES, NO, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
DONE: all events of type <OPERATION-INVOKED-EVENT> which belongs to ASWC IoHwAb or ASWC Aswc_IntDcm must not be mapped TODO: improve offset computing algo
</commit_message>
<xml_diff>
--- a/RTE_Configurator test plan.xlsx
+++ b/RTE_Configurator test plan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristi\PycharmProjects\RTE_Config\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="5940" windowWidth="19260" windowHeight="6000" activeTab="1"/>
   </bookViews>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="123">
   <si>
     <t>Requirements</t>
   </si>
@@ -1168,13 +1173,68 @@
   <si>
     <t xml:space="preserve">- check  in the script that the order is event3, event2,  event1
 </t>
+  </si>
+  <si>
+    <t>All the events of type &lt;OPERATION-INVOKED-EVENT&gt; which belongs to ASWC IoHwAb  or ASWC Aswc_IntDcm mult not be mapped</t>
+  </si>
+  <si>
+    <t>- check that in the output file the event is not found</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Provide to the tool one file havin one event of type &lt;OPERATION-INVOKED-EVENT&gt; assigned to ASWC IoHwAb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Test 1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Provide to the tool one file havin one event of type &lt;OPERATION-INVOKED-EVENT&gt; assigned to ASWC Aswc_IntDcm</t>
+    </r>
+  </si>
+  <si>
+    <t>RTE.EXCEPT.OIE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1553,7 +1613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1708,11 +1768,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1765,6 +1881,14 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2023,28 +2147,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="68.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
@@ -2058,7 +2182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>9</v>
       </c>
@@ -2072,97 +2196,97 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="17"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="10"/>
       <c r="D4" s="9"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="9"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="10"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="10"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
@@ -2175,17 +2299,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D35" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" style="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
@@ -2195,7 +2319,7 @@
     <col min="6" max="6" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -2215,7 +2339,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30.75" thickTop="1">
+    <row r="2" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>29</v>
       </c>
@@ -2235,7 +2359,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>30</v>
       </c>
@@ -2255,7 +2379,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>89</v>
       </c>
@@ -2275,7 +2399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
         <v>33</v>
       </c>
@@ -2295,7 +2419,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>90</v>
       </c>
@@ -2316,7 +2440,7 @@
       </c>
       <c r="G6" s="31"/>
     </row>
-    <row r="7" spans="1:7" ht="60">
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="58"/>
       <c r="B7" s="59"/>
       <c r="C7" s="18" t="s">
@@ -2332,7 +2456,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="60">
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="58"/>
       <c r="B8" s="59"/>
       <c r="C8" s="18" t="s">
@@ -2348,7 +2472,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45">
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="58"/>
       <c r="B9" s="59"/>
       <c r="C9" s="18" t="s">
@@ -2364,7 +2488,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="60">
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
         <v>47</v>
       </c>
@@ -2384,7 +2508,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
         <v>49</v>
       </c>
@@ -2404,7 +2528,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>91</v>
       </c>
@@ -2424,7 +2548,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60.75" customHeight="1">
+    <row r="13" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>92</v>
       </c>
@@ -2444,7 +2568,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="45">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="58"/>
       <c r="B14" s="59"/>
       <c r="C14" s="47" t="s">
@@ -2460,7 +2584,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="65.25" customHeight="1">
+    <row r="15" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="58"/>
       <c r="B15" s="59"/>
       <c r="C15" s="47" t="s">
@@ -2476,7 +2600,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="58"/>
       <c r="B16" s="59"/>
       <c r="C16" s="47" t="s">
@@ -2492,7 +2616,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="58"/>
       <c r="B17" s="59"/>
       <c r="C17" s="47" t="s">
@@ -2508,7 +2632,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="60">
+    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="52" t="s">
         <v>93</v>
       </c>
@@ -2528,7 +2652,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="60">
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="53"/>
       <c r="B19" s="56"/>
       <c r="C19" s="18" t="s">
@@ -2544,7 +2668,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="75">
+    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="53"/>
       <c r="B20" s="56"/>
       <c r="C20" s="37" t="s">
@@ -2560,7 +2684,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="75">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="53"/>
       <c r="B21" s="56"/>
       <c r="C21" s="18" t="s">
@@ -2576,7 +2700,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60">
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="53"/>
       <c r="B22" s="56"/>
       <c r="C22" s="18" t="s">
@@ -2592,7 +2716,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="75">
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="53"/>
       <c r="B23" s="56"/>
       <c r="C23" s="18" t="s">
@@ -2608,7 +2732,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="75">
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="54"/>
       <c r="B24" s="57"/>
       <c r="C24" s="18" t="s">
@@ -2624,7 +2748,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45">
+    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="58" t="s">
         <v>94</v>
       </c>
@@ -2644,7 +2768,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="45">
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="58"/>
       <c r="B26" s="59"/>
       <c r="C26" s="18" t="s">
@@ -2660,7 +2784,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="45">
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="58"/>
       <c r="B27" s="59"/>
       <c r="C27" s="18" t="s">
@@ -2676,7 +2800,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" ht="45">
+    <row r="28" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
         <v>95</v>
       </c>
@@ -2696,7 +2820,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30">
+    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
         <v>64</v>
       </c>
@@ -2716,7 +2840,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="75">
+    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="50" t="s">
         <v>69</v>
       </c>
@@ -2736,7 +2860,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="45">
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="52" t="s">
         <v>86</v>
       </c>
@@ -2756,7 +2880,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="45">
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="53"/>
       <c r="B32" s="56"/>
       <c r="C32" s="46" t="s">
@@ -2772,7 +2896,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="45">
+    <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="53"/>
       <c r="B33" s="56"/>
       <c r="C33" s="46" t="s">
@@ -2788,7 +2912,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="80.25" customHeight="1">
+    <row r="34" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="53"/>
       <c r="B34" s="56"/>
       <c r="C34" s="46" t="s">
@@ -2804,7 +2928,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="60">
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="53"/>
       <c r="B35" s="56"/>
       <c r="C35" s="46" t="s">
@@ -2820,7 +2944,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="75">
+    <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="53"/>
       <c r="B36" s="56"/>
       <c r="C36" s="46" t="s">
@@ -2836,7 +2960,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="75">
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="53"/>
       <c r="B37" s="56"/>
       <c r="C37" s="46" t="s">
@@ -2852,7 +2976,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="75">
+    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="53"/>
       <c r="B38" s="56"/>
       <c r="C38" s="46" t="s">
@@ -2868,7 +2992,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="75">
+    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="54"/>
       <c r="B39" s="57"/>
       <c r="C39" s="46" t="s">
@@ -2884,7 +3008,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="30">
+    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="42" t="s">
         <v>78</v>
       </c>
@@ -2904,54 +3028,92 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="43" t="s">
+    <row r="41" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="61"/>
+      <c r="B42" s="57"/>
+      <c r="C42" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="38" t="s">
+      <c r="B43" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C43" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D43" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E43" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="36" t="s">
+      <c r="F43" s="36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30.75" thickBot="1">
-      <c r="A42" s="44" t="s">
+    <row r="44" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="32" t="s">
+      <c r="B44" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="33" t="s">
+      <c r="C44" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D44" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E44" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="F42" s="36" t="s">
+      <c r="F44" s="36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
-      <c r="B43" s="1" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E29"/>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
     <mergeCell ref="A31:A39"/>
     <mergeCell ref="B31:B39"/>
     <mergeCell ref="A25:A27"/>
@@ -2963,32 +3125,32 @@
     <mergeCell ref="B18:B24"/>
     <mergeCell ref="A18:A24"/>
   </mergeCells>
-  <conditionalFormatting sqref="E46:E1048576 E1:E43">
-    <cfRule type="cellIs" dxfId="4" priority="19" operator="equal">
+  <conditionalFormatting sqref="E48:E1048576 E1:E45">
+    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F42">
-    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
+  <conditionalFormatting sqref="F2:F44">
+    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F42">
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
+  <conditionalFormatting sqref="F2:F44">
+    <cfRule type="cellIs" dxfId="5" priority="17" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E44">
       <formula1>"done, not done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F44">
       <formula1>"YES, NO, N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>